<commit_message>
improvement in evaluation scores controller and logic changed in employee course performance
</commit_message>
<xml_diff>
--- a/Biit Employee Performance Apraisal API/CHR_Excel_Sheet/Book2.xlsx
+++ b/Biit Employee Performance Apraisal API/CHR_Excel_Sheet/Book2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HASSA\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Course</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>OR</t>
+  </si>
+  <si>
+    <t>Fall-2023</t>
   </si>
 </sst>
 </file>
@@ -470,20 +473,20 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -528,8 +531,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -545,8 +551,11 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -562,8 +571,11 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -579,8 +591,11 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -596,8 +611,11 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -613,8 +631,11 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -629,6 +650,9 @@
       </c>
       <c r="E8" t="s">
         <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>